<commit_message>
fix bug es ist ein(s) Uhr
</commit_message>
<xml_diff>
--- a/own/zahlen.xlsx
+++ b/own/zahlen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sören\Documents\wordclock\mywordclock\own\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2B64797-F61A-49C3-A6CF-7CA481AA17D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94CE6D7-5585-4978-984B-B492F52D16C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="40320" windowHeight="17496" xr2:uid="{D313047F-2A21-47A3-BD8A-E2CED2B03AA3}"/>
+    <workbookView xWindow="51480" yWindow="10530" windowWidth="29040" windowHeight="15840" xr2:uid="{D313047F-2A21-47A3-BD8A-E2CED2B03AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,20 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,8 +52,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -54,8 +72,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,16 +86,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -386,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A54BEA0-6CCC-425D-887F-4DC6E3874BE2}">
-  <dimension ref="C1:AN5"/>
+  <dimension ref="C1:AN14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.109375" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -507,6 +554,248 @@
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
     </row>
+    <row r="10" spans="3:40" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V10" s="4">
+        <v>0</v>
+      </c>
+      <c r="W10" s="4">
+        <v>1</v>
+      </c>
+      <c r="X10" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>43</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>42</v>
+      </c>
+      <c r="AB10" s="4">
+        <v>41</v>
+      </c>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4">
+        <v>40</v>
+      </c>
+      <c r="AE10" s="4">
+        <v>39</v>
+      </c>
+      <c r="AF10" s="4">
+        <v>38</v>
+      </c>
+      <c r="AG10" s="4">
+        <v>37</v>
+      </c>
+      <c r="AH10" s="4">
+        <v>36</v>
+      </c>
+      <c r="AI10" s="4">
+        <v>35</v>
+      </c>
+      <c r="AJ10" s="4">
+        <v>34</v>
+      </c>
+      <c r="AK10" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="3:40" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+      <c r="V11" s="4">
+        <v>3</v>
+      </c>
+      <c r="W11" s="4">
+        <v>4</v>
+      </c>
+      <c r="X11" s="4">
+        <v>5</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>44</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>45</v>
+      </c>
+      <c r="AB11" s="4">
+        <v>46</v>
+      </c>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4">
+        <v>47</v>
+      </c>
+      <c r="AE11" s="4">
+        <v>48</v>
+      </c>
+      <c r="AF11" s="4">
+        <v>49</v>
+      </c>
+      <c r="AG11" s="4">
+        <v>50</v>
+      </c>
+      <c r="AH11" s="4">
+        <v>51</v>
+      </c>
+      <c r="AI11" s="4">
+        <v>52</v>
+      </c>
+      <c r="AJ11" s="4">
+        <v>53</v>
+      </c>
+      <c r="AK11" s="4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="3:40" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V12" s="4">
+        <v>6</v>
+      </c>
+      <c r="W12" s="4">
+        <v>7</v>
+      </c>
+      <c r="X12" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>65</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>64</v>
+      </c>
+      <c r="AB12" s="4">
+        <v>63</v>
+      </c>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4">
+        <v>62</v>
+      </c>
+      <c r="AE12" s="4">
+        <v>61</v>
+      </c>
+      <c r="AF12" s="4">
+        <v>60</v>
+      </c>
+      <c r="AG12" s="4">
+        <v>59</v>
+      </c>
+      <c r="AH12" s="4">
+        <v>58</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>57</v>
+      </c>
+      <c r="AJ12" s="4">
+        <v>56</v>
+      </c>
+      <c r="AK12" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="3:40" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+      <c r="V13" s="4">
+        <v>9</v>
+      </c>
+      <c r="W13" s="4">
+        <v>10</v>
+      </c>
+      <c r="X13" s="4">
+        <v>11</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>66</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>67</v>
+      </c>
+      <c r="AB13" s="4">
+        <v>68</v>
+      </c>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4">
+        <v>69</v>
+      </c>
+      <c r="AE13" s="4">
+        <v>70</v>
+      </c>
+      <c r="AF13" s="4">
+        <v>71</v>
+      </c>
+      <c r="AG13" s="4">
+        <v>72</v>
+      </c>
+      <c r="AH13" s="4">
+        <v>73</v>
+      </c>
+      <c r="AI13" s="4">
+        <v>74</v>
+      </c>
+      <c r="AJ13" s="4">
+        <v>75</v>
+      </c>
+      <c r="AK13" s="4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="3:40" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V14" s="4">
+        <v>12</v>
+      </c>
+      <c r="W14" s="4">
+        <v>13</v>
+      </c>
+      <c r="X14" s="4">
+        <v>14</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>87</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>86</v>
+      </c>
+      <c r="AB14" s="4">
+        <v>85</v>
+      </c>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4">
+        <v>84</v>
+      </c>
+      <c r="AE14" s="4">
+        <v>83</v>
+      </c>
+      <c r="AF14" s="4">
+        <v>82</v>
+      </c>
+      <c r="AG14" s="4">
+        <v>81</v>
+      </c>
+      <c r="AH14" s="4">
+        <v>80</v>
+      </c>
+      <c r="AI14" s="4">
+        <v>79</v>
+      </c>
+      <c r="AJ14" s="4">
+        <v>78</v>
+      </c>
+      <c r="AK14" s="4">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>